<commit_message>
fix adorator info download + some sonar issues
</commit_message>
<xml_diff>
--- a/config/security/daily_info.xlsx
+++ b/config/security/daily_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\adoration\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C52EC-DB0C-4203-9845-1820C65B8557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D6149C-9491-4897-A09F-090B5E56BCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0455A818-22EF-4517-BB38-855DBC0A67FD}"/>
+    <workbookView xWindow="1020" yWindow="570" windowWidth="26580" windowHeight="11385" xr2:uid="{0455A818-22EF-4517-BB38-855DBC0A67FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hajnal" sheetId="5" r:id="rId1"/>
@@ -746,8 +746,8 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5719,7 +5719,7 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>